<commit_message>
Format graphs in result spreadsheet for use in report
</commit_message>
<xml_diff>
--- a/doc/results.xlsx
+++ b/doc/results.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\TAE\EE5616\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\TAE\EE5616\EE5616_1841781\src\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384"/>
   </bookViews>
   <sheets>
     <sheet name="resultGetxGetY" sheetId="2" r:id="rId1"/>
@@ -627,6 +627,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1063,11 +1064,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="381211704"/>
-        <c:axId val="381211312"/>
+        <c:axId val="402772792"/>
+        <c:axId val="402773184"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="381211704"/>
+        <c:axId val="402772792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1110,7 +1111,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="381211312"/>
+        <c:crossAx val="402773184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1118,7 +1119,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="381211312"/>
+        <c:axId val="402773184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1169,7 +1170,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="381211704"/>
+        <c:crossAx val="402772792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1183,6 +1184,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1725,11 +1727,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="379380280"/>
-        <c:axId val="190253440"/>
+        <c:axId val="402772400"/>
+        <c:axId val="402773576"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="379380280"/>
+        <c:axId val="402772400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1772,7 +1774,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="190253440"/>
+        <c:crossAx val="402773576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1780,7 +1782,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="190253440"/>
+        <c:axId val="402773576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1831,7 +1833,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="379380280"/>
+        <c:crossAx val="402772400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1922,6 +1924,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2162,11 +2165,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="424692864"/>
-        <c:axId val="424694040"/>
+        <c:axId val="402773968"/>
+        <c:axId val="402774752"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="424692864"/>
+        <c:axId val="402773968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2209,7 +2212,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="424694040"/>
+        <c:crossAx val="402774752"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2217,7 +2220,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="424694040"/>
+        <c:axId val="402774752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2268,7 +2271,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="424692864"/>
+        <c:crossAx val="402773968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2578,11 +2581,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="424693256"/>
-        <c:axId val="424693648"/>
+        <c:axId val="402777104"/>
+        <c:axId val="189564840"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="424693256"/>
+        <c:axId val="402777104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2625,7 +2628,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="424693648"/>
+        <c:crossAx val="189564840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2633,7 +2636,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="424693648"/>
+        <c:axId val="189564840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2684,7 +2687,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="424693256"/>
+        <c:crossAx val="402777104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4956,7 +4959,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="93" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="93" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4989,7 +4992,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="93" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="93" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5000,7 +5003,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9283290" cy="6063226"/>
+    <xdr:ext cx="9283290" cy="6055032"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -5054,7 +5057,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9283290" cy="6063226"/>
+    <xdr:ext cx="9283290" cy="6055032"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>

</xml_diff>